<commit_message>
mm and inch planned for 2023
</commit_message>
<xml_diff>
--- a/docs/CHILI-GraFx/applications/comparison/features.xlsx
+++ b/docs/CHILI-GraFx/applications/comparison/features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bram/Documents/GitHub/grafx-documentation/docs/CHILI-GraFx/applications/comparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDCFCED-9A87-9646-B743-D89EDB149258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6D5DC-6D33-1B48-8442-901E0A92163D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11680" yWindow="640" windowWidth="20480" windowHeight="19520" xr2:uid="{BF9F8A34-DC7E-0549-A389-ADCA54F02979}"/>
   </bookViews>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26496501-D774-604E-8805-246C457AC686}">
   <dimension ref="A1:D174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:XFD73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1283,7 +1283,7 @@
         <v>183</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>135</v>
+        <v>188</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>132</v>
@@ -1297,7 +1297,7 @@
         <v>184</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>135</v>
+        <v>188</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>132</v>

</xml_diff>